<commit_message>
Simple Gantt Update 25
Simple Gantt Update 25
</commit_message>
<xml_diff>
--- a/Civilworks cost/Work Schedule/Schdule Input.xlsx
+++ b/Civilworks cost/Work Schedule/Schdule Input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -515,7 +515,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -529,13 +529,13 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -552,7 +552,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -567,7 +567,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -584,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -601,7 +601,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -618,7 +618,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -635,7 +635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -674,14 +674,14 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -698,7 +698,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -715,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -732,7 +732,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -749,7 +749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -766,7 +766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -783,7 +783,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -800,7 +800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -817,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -834,7 +834,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -865,14 +865,14 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.109375" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" customWidth="1"/>
-    <col min="4" max="4" width="38.33203125" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -886,7 +886,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -900,7 +900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>22</v>
       </c>
@@ -914,12 +914,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -934,17 +934,17 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -964,7 +964,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -984,7 +984,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>33338</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>5012</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>6974</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>6098</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>38350</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1175,17 +1175,17 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1245,7 +1245,7 @@
         <v>1188</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1265,7 +1265,7 @@
         <v>7900</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1305,7 +1305,7 @@
         <v>1653</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1313,7 +1313,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4">
         <v>5</v>
@@ -1325,7 +1325,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1333,7 +1333,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D8" s="4">
         <v>6</v>
@@ -1345,7 +1345,7 @@
         <v>1445</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D9" s="4">
         <v>7</v>
@@ -1365,7 +1365,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>31</v>
@@ -1385,7 +1385,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1419,14 +1419,14 @@
       <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>4151</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1640,14 +1640,14 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="2" max="2" width="33.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>4151</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1747,7 +1747,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Simple Gantt Chart Update 50
Simple Gantt Chart Update 50
</commit_message>
<xml_diff>
--- a/Civilworks cost/Work Schedule/Schdule Input.xlsx
+++ b/Civilworks cost/Work Schedule/Schdule Input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -133,6 +133,15 @@
   </si>
   <si>
     <t>Curing</t>
+  </si>
+  <si>
+    <t>Site Name</t>
+  </si>
+  <si>
+    <t>Type A slope protection work of the Dharmapasha Ruibeel Submergible Embankment from M724  to M935=935M</t>
+  </si>
+  <si>
+    <t>Type A slope protection work of the Dharmapasha Ruibeel Submergible Embankment from M965  to M1015=50M</t>
   </si>
 </sst>
 </file>
@@ -168,7 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -191,19 +200,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -222,14 +218,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -859,10 +857,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,9 +868,10 @@
     <col min="1" max="1" width="32.140625" customWidth="1"/>
     <col min="3" max="3" width="6.7109375" customWidth="1"/>
     <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="5" max="5" width="57.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -885,8 +884,11 @@
       <c r="D1" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>21</v>
       </c>
@@ -896,12 +898,15 @@
       <c r="C2" s="4">
         <v>87</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="E2" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B3" s="4">
@@ -913,16 +918,19 @@
       <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="E3" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -968,7 +976,7 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4">
@@ -988,7 +996,7 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4">
@@ -1008,7 +1016,7 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4">
@@ -1028,7 +1036,7 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>29</v>
       </c>
       <c r="C5" s="4">
@@ -1048,7 +1056,7 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4">
@@ -1068,7 +1076,7 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4">
@@ -1088,7 +1096,7 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4">
@@ -1108,7 +1116,7 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4">
@@ -1128,7 +1136,7 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="4">
@@ -1148,7 +1156,7 @@
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4">
@@ -1174,7 +1182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -1209,7 +1217,7 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4">
@@ -1221,7 +1229,7 @@
       <c r="E2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="7">
         <v>100</v>
       </c>
     </row>
@@ -1229,7 +1237,7 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4">
@@ -1241,7 +1249,7 @@
       <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>1188</v>
       </c>
     </row>
@@ -1249,7 +1257,7 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4">
@@ -1261,7 +1269,7 @@
       <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>7900</v>
       </c>
     </row>
@@ -1269,7 +1277,7 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C5" s="4">
@@ -1281,7 +1289,7 @@
       <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>100</v>
       </c>
     </row>
@@ -1289,7 +1297,7 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="4">
@@ -1301,7 +1309,7 @@
       <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>1653</v>
       </c>
     </row>
@@ -1309,7 +1317,7 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4">
@@ -1321,7 +1329,7 @@
       <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>133</v>
       </c>
     </row>
@@ -1329,7 +1337,7 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="4">
@@ -1341,7 +1349,7 @@
       <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>1445</v>
       </c>
     </row>
@@ -1349,7 +1357,7 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="4">
@@ -1361,7 +1369,7 @@
       <c r="E9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>133</v>
       </c>
     </row>
@@ -1369,7 +1377,7 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C10" s="4">
@@ -1381,7 +1389,7 @@
       <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>328</v>
       </c>
     </row>
@@ -1389,7 +1397,7 @@
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="4">
@@ -1401,7 +1409,7 @@
       <c r="E11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>100</v>
       </c>
     </row>
@@ -1450,7 +1458,7 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4">
@@ -1470,7 +1478,7 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4">
@@ -1482,7 +1490,7 @@
       <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>950</v>
       </c>
     </row>
@@ -1490,7 +1498,7 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4">
@@ -1502,7 +1510,7 @@
       <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>4151</v>
       </c>
     </row>
@@ -1510,7 +1518,7 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4">
@@ -1522,7 +1530,7 @@
       <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>330</v>
       </c>
     </row>
@@ -1530,7 +1538,7 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4">
@@ -1542,7 +1550,7 @@
       <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>68</v>
       </c>
     </row>
@@ -1550,7 +1558,7 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4">
@@ -1562,7 +1570,7 @@
       <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>770</v>
       </c>
     </row>
@@ -1570,7 +1578,7 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4">
@@ -1582,7 +1590,7 @@
       <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>68</v>
       </c>
     </row>
@@ -1590,7 +1598,7 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="4">
@@ -1602,7 +1610,7 @@
       <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>193</v>
       </c>
     </row>
@@ -1610,7 +1618,7 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="4">
@@ -1671,7 +1679,7 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="4">
@@ -1691,7 +1699,7 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="4">
@@ -1703,7 +1711,7 @@
       <c r="E3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="7">
         <v>950</v>
       </c>
     </row>
@@ -1711,7 +1719,7 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4">
@@ -1723,7 +1731,7 @@
       <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>4151</v>
       </c>
     </row>
@@ -1731,7 +1739,7 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="4">
@@ -1743,7 +1751,7 @@
       <c r="E5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="7">
         <v>330</v>
       </c>
     </row>
@@ -1751,7 +1759,7 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4">
@@ -1763,7 +1771,7 @@
       <c r="E6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>68</v>
       </c>
     </row>
@@ -1771,7 +1779,7 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="4">
@@ -1783,7 +1791,7 @@
       <c r="E7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="7">
         <v>770</v>
       </c>
     </row>
@@ -1791,7 +1799,7 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4">
@@ -1803,7 +1811,7 @@
       <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>68</v>
       </c>
     </row>
@@ -1811,7 +1819,7 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="4">
@@ -1823,7 +1831,7 @@
       <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>193</v>
       </c>
     </row>
@@ -1831,7 +1839,7 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="4">

</xml_diff>